<commit_message>
eda pof e pam
</commit_message>
<xml_diff>
--- a/pam_alimentos_cesta.xlsx
+++ b/pam_alimentos_cesta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dcc-fellowship-ciencia-de-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD5086D-23D8-4D17-9DE0-4161DBE190DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7CE7D7-D4C0-43F1-8937-236E95D470D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Ano</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>MIlho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arroz </t>
+  </si>
+  <si>
+    <t>Café (em grão)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -471,10 +477,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>5</v>

</xml_diff>